<commit_message>
Fixed time & Actualize with Matlab
</commit_message>
<xml_diff>
--- a/time_sheet.xlsx
+++ b/time_sheet.xlsx
@@ -146,7 +146,7 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Mô hình máy bay trên máy tinh. Hiểu các thông số điều khiển. Khả năng của Matlab</t>
+Mô hình máy bay trên máy tính. Hiểu các thông số điều khiển. Xuất code nhúng cho các module</t>
         </r>
       </text>
     </comment>
@@ -2260,9 +2260,9 @@
   </sheetPr>
   <dimension ref="A1:NK52"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" sqref="A1:H1"/>
+      <selection pane="topRight" activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.42578125" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>

</xml_diff>